<commit_message>
Added nelder-mead based OPF to dispatch batteries (still work to do)
</commit_message>
<xml_diff>
--- a/Grids_and_profiles/grids/IEEE 30 Bus with storage.xlsx
+++ b/Grids_and_profiles/grids/IEEE 30 Bus with storage.xlsx
@@ -119,10 +119,10 @@
     <t>0j</t>
   </si>
   <si>
-    <t>-19525.0</t>
-  </si>
-  <si>
-    <t>-10305.0</t>
+    <t>-19892.0</t>
+  </si>
+  <si>
+    <t>-10498.0</t>
   </si>
   <si>
     <t>20.0</t>
@@ -146,19 +146,19 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>-19103.0</t>
-  </si>
-  <si>
-    <t>-10343.0</t>
+    <t>-19470.0</t>
+  </si>
+  <si>
+    <t>-10536.0</t>
   </si>
   <si>
     <t>bus 2</t>
   </si>
   <si>
-    <t>-19410.0</t>
-  </si>
-  <si>
-    <t>-10612.0</t>
+    <t>-19777.0</t>
+  </si>
+  <si>
+    <t>-10805.0</t>
   </si>
   <si>
     <t>bus 3</t>
@@ -167,106 +167,106 @@
     <t>bus 4</t>
   </si>
   <si>
-    <t>-18987.0</t>
-  </si>
-  <si>
-    <t>-10151.0</t>
+    <t>-19354.0</t>
+  </si>
+  <si>
+    <t>-10344.0</t>
   </si>
   <si>
     <t>bus 5</t>
   </si>
   <si>
-    <t>-18757.0</t>
-  </si>
-  <si>
-    <t>-10459.0</t>
+    <t>-19124.0</t>
+  </si>
+  <si>
+    <t>-10652.0</t>
   </si>
   <si>
     <t>bus 6</t>
   </si>
   <si>
-    <t>-18833.0</t>
-  </si>
-  <si>
-    <t>-10228.0</t>
+    <t>-19200.0</t>
+  </si>
+  <si>
+    <t>-10421.0</t>
   </si>
   <si>
     <t>bus 7</t>
   </si>
   <si>
-    <t>-18680.0</t>
-  </si>
-  <si>
-    <t>-10189.0</t>
+    <t>-19047.0</t>
+  </si>
+  <si>
+    <t>-10382.0</t>
   </si>
   <si>
     <t>bus 8</t>
   </si>
   <si>
-    <t>-18603.0</t>
-  </si>
-  <si>
-    <t>-10497.0</t>
+    <t>-18970.0</t>
+  </si>
+  <si>
+    <t>-10690.0</t>
   </si>
   <si>
     <t>bus 9</t>
   </si>
   <si>
-    <t>-10689.0</t>
+    <t>-10882.0</t>
   </si>
   <si>
     <t>bus 10</t>
   </si>
   <si>
-    <t>-18411.0</t>
-  </si>
-  <si>
-    <t>-10420.0</t>
+    <t>-18778.0</t>
+  </si>
+  <si>
+    <t>-10613.0</t>
   </si>
   <si>
     <t>bus 11</t>
   </si>
   <si>
-    <t>-19064.0</t>
-  </si>
-  <si>
-    <t>-10881.0</t>
+    <t>-19431.0</t>
+  </si>
+  <si>
+    <t>-11074.0</t>
   </si>
   <si>
     <t>bus 12</t>
   </si>
   <si>
-    <t>-19372.0</t>
-  </si>
-  <si>
-    <t>-10766.0</t>
+    <t>-19739.0</t>
+  </si>
+  <si>
+    <t>-10959.0</t>
   </si>
   <si>
     <t>bus 13</t>
   </si>
   <si>
-    <t>-19295.0</t>
-  </si>
-  <si>
-    <t>-11151.0</t>
+    <t>-19662.0</t>
+  </si>
+  <si>
+    <t>-11344.0</t>
   </si>
   <si>
     <t>bus 14</t>
   </si>
   <si>
-    <t>-18641.0</t>
-  </si>
-  <si>
-    <t>-11343.0</t>
+    <t>-19008.0</t>
+  </si>
+  <si>
+    <t>-11536.0</t>
   </si>
   <si>
     <t>bus 15</t>
   </si>
   <si>
-    <t>-18910.0</t>
-  </si>
-  <si>
-    <t>-10805.0</t>
+    <t>-19277.0</t>
+  </si>
+  <si>
+    <t>-10998.0</t>
   </si>
   <si>
     <t>bus 16</t>
@@ -275,31 +275,31 @@
     <t>bus 17</t>
   </si>
   <si>
-    <t>-18718.0</t>
-  </si>
-  <si>
-    <t>-11074.0</t>
+    <t>-19085.0</t>
+  </si>
+  <si>
+    <t>-11267.0</t>
   </si>
   <si>
     <t>bus 18</t>
   </si>
   <si>
-    <t>-10920.0</t>
+    <t>-11113.0</t>
   </si>
   <si>
     <t>bus 19</t>
   </si>
   <si>
-    <t>-10728.0</t>
+    <t>-10921.0</t>
   </si>
   <si>
     <t>bus 20</t>
   </si>
   <si>
-    <t>-18372.0</t>
-  </si>
-  <si>
-    <t>-10651.0</t>
+    <t>-18739.0</t>
+  </si>
+  <si>
+    <t>-10844.0</t>
   </si>
   <si>
     <t>bus 21</t>
@@ -308,58 +308,58 @@
     <t>bus 22</t>
   </si>
   <si>
-    <t>-18449.0</t>
-  </si>
-  <si>
-    <t>-11112.0</t>
+    <t>-18816.0</t>
+  </si>
+  <si>
+    <t>-11305.0</t>
   </si>
   <si>
     <t>bus 23</t>
   </si>
   <si>
-    <t>-18141.0</t>
-  </si>
-  <si>
-    <t>-11035.0</t>
+    <t>-18508.0</t>
+  </si>
+  <si>
+    <t>-11228.0</t>
   </si>
   <si>
     <t>bus 24</t>
   </si>
   <si>
-    <t>-18103.0</t>
+    <t>-18470.0</t>
   </si>
   <si>
     <t>bus 25</t>
   </si>
   <si>
-    <t>-17603.0</t>
+    <t>-17970.0</t>
   </si>
   <si>
     <t>bus 26</t>
   </si>
   <si>
-    <t>-18218.0</t>
+    <t>-18585.0</t>
   </si>
   <si>
     <t>bus 27</t>
   </si>
   <si>
-    <t>-18564.0</t>
+    <t>-18931.0</t>
   </si>
   <si>
     <t>bus 28</t>
   </si>
   <si>
-    <t>-18065.0</t>
-  </si>
-  <si>
-    <t>-10036.0</t>
+    <t>-18432.0</t>
+  </si>
+  <si>
+    <t>-10229.0</t>
   </si>
   <si>
     <t>bus 29</t>
   </si>
   <si>
-    <t>-17834.0</t>
+    <t>-18201.0</t>
   </si>
   <si>
     <t>bus_from</t>
@@ -6593,7 +6593,7 @@
     <t>discharge_efficiency</t>
   </si>
   <si>
-    <t>batt</t>
+    <t>batt1@bus 5</t>
   </si>
   <si>
     <t>batt1@bus 13</t>
@@ -6702,9 +6702,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -6750,7 +6749,7 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -7209,10 +7208,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>9999</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>9999</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
         <v>-9999</v>
@@ -7221,10 +7220,10 @@
         <v>9999</v>
       </c>
       <c r="K2" t="n">
-        <v>-9999</v>
+        <v>-1</v>
       </c>
       <c r="L2" t="n">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -9586,7 +9585,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -9633,7 +9632,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -9727,7 +9726,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -9774,7 +9773,7 @@
         <v>1</v>
       </c>
       <c r="M6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -9821,7 +9820,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>

</xml_diff>